<commit_message>
Creo que ya quedó
</commit_message>
<xml_diff>
--- a/precios_historicos_cierre.xlsx
+++ b/precios_historicos_cierre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Marco\Documents\Visual Studio Code Local\Escuela VS\Concentracion Economia y Finanzas\Riesgos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0594DDE3-FB8C-4925-81BA-70CBCD7777AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7CEB5F-007E-4AD9-A94E-AE44438CC604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>005930.KS Usd</t>
+  </si>
+  <si>
+    <t>Valor Portafolio</t>
+  </si>
+  <si>
+    <t>Rendimiento portafolio</t>
   </si>
 </sst>
 </file>
@@ -479,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1063"/>
+  <dimension ref="A1:P1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1049" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K1063" sqref="K1063"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -499,7 +505,7 @@
     <col min="11" max="11" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,8 +548,14 @@
       <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45994</v>
       </c>
@@ -586,8 +598,14 @@
       <c r="N2">
         <v>311.32435897435897</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>1009012.0499999999</v>
+      </c>
+      <c r="P2">
+        <v>9.0120499999999382E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45993</v>
       </c>
@@ -631,8 +649,14 @@
       <c r="N3">
         <v>307.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3">
+        <v>1005538.5115100001</v>
+      </c>
+      <c r="P3">
+        <v>5.5385115100001769E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45992</v>
       </c>
@@ -676,8 +700,14 @@
       <c r="N4">
         <v>308.92</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>993871.23579999991</v>
+      </c>
+      <c r="P4">
+        <v>-6.1287642000000808E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45989</v>
       </c>
@@ -721,8 +751,14 @@
       <c r="N5">
         <v>313.08</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5">
+        <v>994786.57065000001</v>
+      </c>
+      <c r="P5">
+        <v>-5.2134293500000206E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45987</v>
       </c>
@@ -766,8 +802,14 @@
       <c r="N6">
         <v>307.64</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6">
+        <v>992596.57265999995</v>
+      </c>
+      <c r="P6">
+        <v>-7.4034273400001016E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45986</v>
       </c>
@@ -811,8 +853,14 @@
       <c r="N7">
         <v>303</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7">
+        <v>984834.50469999993</v>
+      </c>
+      <c r="P7">
+        <v>-1.5165495300000109E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45985</v>
       </c>
@@ -856,8 +904,14 @@
       <c r="N8">
         <v>298</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8">
+        <v>988318.42399999988</v>
+      </c>
+      <c r="P8">
+        <v>-1.1681576000000082E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45982</v>
       </c>
@@ -901,8 +955,14 @@
       <c r="N9">
         <v>298.02</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9">
+        <v>969591.16548499989</v>
+      </c>
+      <c r="P9">
+        <v>-3.0408834515000094E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45981</v>
       </c>
@@ -946,8 +1006,14 @@
       <c r="N10">
         <v>298.38</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>968949.04692999984</v>
+      </c>
+      <c r="P10">
+        <v>-3.1050953070000165E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45980</v>
       </c>
@@ -991,8 +1057,14 @@
       <c r="N11">
         <v>303.27</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11">
+        <v>985851.79823999992</v>
+      </c>
+      <c r="P11">
+        <v>-1.414820176000009E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45979</v>
       </c>
@@ -1036,8 +1108,14 @@
       <c r="N12">
         <v>299.41000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>973542.52156500006</v>
+      </c>
+      <c r="P12">
+        <v>-2.6457478434999904E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45978</v>
       </c>
@@ -1081,8 +1159,14 @@
       <c r="N13">
         <v>300.37</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>988132.40299999993</v>
+      </c>
+      <c r="P13">
+        <v>-1.1867597000000063E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45975</v>
       </c>
@@ -1126,8 +1210,14 @@
       <c r="N14">
         <v>303.61</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14">
+        <v>998547.40229999996</v>
+      </c>
+      <c r="P14">
+        <v>-1.4525977000000578E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45974</v>
       </c>
@@ -1171,8 +1261,14 @@
       <c r="N15">
         <v>309.48</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15">
+        <v>989904.7453000003</v>
+      </c>
+      <c r="P15">
+        <v>-1.0095254699999723E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45973</v>
       </c>
@@ -1216,8 +1312,14 @@
       <c r="N16">
         <v>320.41000000000003</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>1021011.2479200001</v>
+      </c>
+      <c r="P16">
+        <v>2.1011247920000198E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45972</v>
       </c>
@@ -1261,8 +1363,14 @@
       <c r="N17">
         <v>315.62</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17">
+        <v>1018026.0348000001</v>
+      </c>
+      <c r="P17">
+        <v>1.802603480000009E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45971</v>
       </c>
@@ -1306,8 +1414,14 @@
       <c r="N18">
         <v>316.89</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18">
+        <v>1020399.3194800002</v>
+      </c>
+      <c r="P18">
+        <v>2.0399319480000289E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45968</v>
       </c>
@@ -1351,8 +1465,14 @@
       <c r="N19">
         <v>314.20999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19">
+        <v>1000703.4490500001</v>
+      </c>
+      <c r="P19">
+        <v>7.0344904999997127E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45967</v>
       </c>
@@ -1396,8 +1516,14 @@
       <c r="N20">
         <v>313.42</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>1007470.64688</v>
+      </c>
+      <c r="P20">
+        <v>7.470646880000098E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45966</v>
       </c>
@@ -1441,8 +1567,14 @@
       <c r="N21">
         <v>311.68</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O21">
+        <v>1014830.8554999999</v>
+      </c>
+      <c r="P21">
+        <v>1.4830855499999851E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45965</v>
       </c>
@@ -1486,8 +1618,14 @@
       <c r="N22">
         <v>309.25</v>
       </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O22">
+        <v>1011709.4423600001</v>
+      </c>
+      <c r="P22">
+        <v>1.1709442360000155E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45964</v>
       </c>
@@ -1531,8 +1669,14 @@
       <c r="N23">
         <v>309.35000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O23">
+        <v>1034713.04024</v>
+      </c>
+      <c r="P23">
+        <v>3.4713040239999993E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45961</v>
       </c>
@@ -1576,8 +1720,14 @@
       <c r="N24">
         <v>311.12</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1030279.8677300001</v>
+      </c>
+      <c r="P24">
+        <v>3.0279867730000021E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45960</v>
       </c>
@@ -1621,8 +1771,14 @@
       <c r="N25">
         <v>309.44</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O25">
+        <v>1033525.3895</v>
+      </c>
+      <c r="P25">
+        <v>3.3525389500000058E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45959</v>
       </c>
@@ -1666,8 +1822,14 @@
       <c r="N26">
         <v>305.51</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <v>1042131.1715249999</v>
+      </c>
+      <c r="P26">
+        <v>4.21311715249999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45958</v>
       </c>
@@ -1711,8 +1873,14 @@
       <c r="N27">
         <v>305.36</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <v>1041551.43535</v>
+      </c>
+      <c r="P27">
+        <v>4.1551435349999943E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45957</v>
       </c>
@@ -1756,8 +1924,14 @@
       <c r="N28">
         <v>304.14999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <v>1010144.15246</v>
+      </c>
+      <c r="P28">
+        <v>1.0144152460000111E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45954</v>
       </c>
@@ -1801,8 +1975,14 @@
       <c r="N29">
         <v>300.44</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <v>1048635.4878999998</v>
+      </c>
+      <c r="P29">
+        <v>4.8635487899999941E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45953</v>
       </c>
@@ -1846,8 +2026,14 @@
       <c r="N30">
         <v>294.54000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <v>1046440.1600449999</v>
+      </c>
+      <c r="P30">
+        <v>4.6440160044999956E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45952</v>
       </c>
@@ -1891,8 +2077,14 @@
       <c r="N31">
         <v>294.11</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <v>1027997.4480000001</v>
+      </c>
+      <c r="P31">
+        <v>2.7997448000000036E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45951</v>
       </c>
@@ -1936,8 +2128,14 @@
       <c r="N32">
         <v>297.08999999999997</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <v>1029844.5362799999</v>
+      </c>
+      <c r="P32">
+        <v>2.9844536279999945E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45950</v>
       </c>
@@ -1981,8 +2179,14 @@
       <c r="N33">
         <v>302.36</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <v>1048988.8352999999</v>
+      </c>
+      <c r="P33">
+        <v>4.8988835299999867E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45947</v>
       </c>
@@ -2026,8 +2230,14 @@
       <c r="N34">
         <v>297.56</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>1031171.64591</v>
+      </c>
+      <c r="P34">
+        <v>3.117164590999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45946</v>
       </c>
@@ -2071,8 +2281,14 @@
       <c r="N35">
         <v>298.54000000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <v>1048722.8860749998</v>
+      </c>
+      <c r="P35">
+        <v>4.8722886074999749E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45945</v>
       </c>
@@ -2116,8 +2332,14 @@
       <c r="N36">
         <v>305.69</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <v>1056389.2367100001</v>
+      </c>
+      <c r="P36">
+        <v>5.6389236710000068E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45944</v>
       </c>
@@ -2161,8 +2383,14 @@
       <c r="N37">
         <v>302.08</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <v>1029066.9268750001</v>
+      </c>
+      <c r="P37">
+        <v>2.9066926875000121E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45943</v>
       </c>
@@ -2206,8 +2434,14 @@
       <c r="N38">
         <v>307.97000000000003</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <v>1037036.0438852198</v>
+      </c>
+      <c r="P38">
+        <v>3.7036043885219749E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45940</v>
       </c>
@@ -2251,8 +2485,14 @@
       <c r="N39">
         <v>300.89</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39">
+        <v>1022839.7718148131</v>
+      </c>
+      <c r="P39">
+        <v>2.2839771814813226E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45939</v>
       </c>
@@ -2296,8 +2536,14 @@
       <c r="N40">
         <v>305.52999999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O40">
+        <v>1038873.0265182536</v>
+      </c>
+      <c r="P40">
+        <v>3.8873026518253528E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45938</v>
       </c>
@@ -2341,8 +2587,14 @@
       <c r="N41">
         <v>304.02999999999997</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O41">
+        <v>1048729.6281028164</v>
+      </c>
+      <c r="P41">
+        <v>4.8729628102816447E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45937</v>
       </c>
@@ -2386,8 +2638,14 @@
       <c r="N42">
         <v>307.69</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>1041284.3718249835</v>
+      </c>
+      <c r="P42">
+        <v>4.1284371824983568E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45936</v>
       </c>
@@ -2431,8 +2689,14 @@
       <c r="N43">
         <v>309.18</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O43">
+        <v>1047881.7156686981</v>
+      </c>
+      <c r="P43">
+        <v>4.7881715668698144E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45933</v>
       </c>
@@ -2476,8 +2740,14 @@
       <c r="N44">
         <v>310.02999999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O44">
+        <v>1040317.4159010525</v>
+      </c>
+      <c r="P44">
+        <v>4.0317415901052422E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45932</v>
       </c>
@@ -2521,8 +2791,14 @@
       <c r="N45">
         <v>307.55</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O45">
+        <v>1039768.0166007036</v>
+      </c>
+      <c r="P45">
+        <v>3.9768016600703504E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45931</v>
       </c>
@@ -2566,8 +2842,14 @@
       <c r="N46">
         <v>310.70999999999998</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O46">
+        <v>1038672.1494013753</v>
+      </c>
+      <c r="P46">
+        <v>3.8672149401375311E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45930</v>
       </c>
@@ -2611,8 +2893,14 @@
       <c r="N47">
         <v>315.43</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O47">
+        <v>1042312.7629008521</v>
+      </c>
+      <c r="P47">
+        <v>4.2312762900852174E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45929</v>
       </c>
@@ -2656,8 +2944,14 @@
       <c r="N48">
         <v>315.69</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O48">
+        <v>1035016.338468098</v>
+      </c>
+      <c r="P48">
+        <v>3.5016338468097929E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45926</v>
       </c>
@@ -2701,8 +2995,14 @@
       <c r="N49">
         <v>316.06</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O49">
+        <v>1037262.2762350574</v>
+      </c>
+      <c r="P49">
+        <v>3.7262276235057401E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45925</v>
       </c>
@@ -2746,8 +3046,14 @@
       <c r="N50">
         <v>313.45</v>
       </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O50">
+        <v>1024276.1044040123</v>
+      </c>
+      <c r="P50">
+        <v>2.4276104404012289E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45924</v>
       </c>
@@ -2791,8 +3097,14 @@
       <c r="N51">
         <v>313.42</v>
       </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O51">
+        <v>1023474.6708796474</v>
+      </c>
+      <c r="P51">
+        <v>2.3474670879647386E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45923</v>
       </c>
@@ -2836,8 +3148,14 @@
       <c r="N52">
         <v>312.74</v>
       </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O52">
+        <v>1031008.6359330035</v>
+      </c>
+      <c r="P52">
+        <v>3.1008635933003514E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45922</v>
       </c>
@@ -2881,8 +3199,14 @@
       <c r="N53">
         <v>312.44</v>
       </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O53">
+        <v>1028046.8566955921</v>
+      </c>
+      <c r="P53">
+        <v>2.8046856695592037E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45919</v>
       </c>
@@ -2926,8 +3250,14 @@
       <c r="N54">
         <v>314.77999999999997</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O54">
+        <v>1021789.9348288876</v>
+      </c>
+      <c r="P54">
+        <v>2.1789934828887469E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45918</v>
       </c>
@@ -2971,8 +3301,14 @@
       <c r="N55">
         <v>313.23</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O55">
+        <v>1015213.3932147308</v>
+      </c>
+      <c r="P55">
+        <v>1.5213393214730697E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45917</v>
       </c>
@@ -3016,8 +3352,14 @@
       <c r="N56">
         <v>311.75</v>
       </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O56">
+        <v>1009378.0619924406</v>
+      </c>
+      <c r="P56">
+        <v>9.3780619924406228E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45916</v>
       </c>
@@ -3061,8 +3403,14 @@
       <c r="N57">
         <v>309.19</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O57">
+        <v>1013105.6183529601</v>
+      </c>
+      <c r="P57">
+        <v>1.3105618352960091E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45915</v>
       </c>
@@ -3106,8 +3454,14 @@
       <c r="N58">
         <v>308.89999999999998</v>
       </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O58">
+        <v>1014452.251432293</v>
+      </c>
+      <c r="P58">
+        <v>1.4452251432292895E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45912</v>
       </c>
@@ -3151,8 +3505,14 @@
       <c r="N59">
         <v>306.91000000000003</v>
       </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O59">
+        <v>1006741.9951608838</v>
+      </c>
+      <c r="P59">
+        <v>6.7419951608838069E-3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45911</v>
       </c>
@@ -3196,8 +3556,14 @@
       <c r="N60">
         <v>305.56</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O60">
+        <v>1007074.4843806523</v>
+      </c>
+      <c r="P60">
+        <v>7.0744843806522795E-3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45910</v>
       </c>
@@ -3241,8 +3607,14 @@
       <c r="N61">
         <v>300.54000000000002</v>
       </c>
-    </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O61">
+        <v>1005415.5395581771</v>
+      </c>
+      <c r="P61">
+        <v>5.4155395581771959E-3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45909</v>
       </c>
@@ -3286,8 +3658,14 @@
       <c r="N62">
         <v>297.85000000000002</v>
       </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O62">
+        <v>1001032.0748945731</v>
+      </c>
+      <c r="P62">
+        <v>1.0320748945731317E-3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45908</v>
       </c>
@@ -3331,8 +3709,14 @@
       <c r="N63">
         <v>292.91000000000003</v>
       </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O63">
+        <v>999695.66570694</v>
+      </c>
+      <c r="P63">
+        <v>-3.0433429305998239E-4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45905</v>
       </c>
@@ -46555,7 +46939,7 @@
         <v>145.58000000000001</v>
       </c>
       <c r="H1024">
-        <f t="shared" ref="H1024:H1063" si="16">G1024*K1024</f>
+        <f t="shared" ref="H1024:H1062" si="16">G1024*K1024</f>
         <v>168.37782800000002</v>
       </c>
       <c r="I1024">

</xml_diff>